<commit_message>
add: UTS Implementasi Stok dan Penjualan
</commit_message>
<xml_diff>
--- a/public/template_kategori.xlsx
+++ b/public/template_kategori.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EC65D3C-F3EA-4CB5-965D-51064A8582B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B2A9F-780A-4114-AD52-E597C01DD820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{C19A822D-A30A-4EC7-82A8-78B9589523E6}"/>
+    <workbookView xWindow="5292" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{C19A822D-A30A-4EC7-82A8-78B9589523E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>kategori_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>kategori_kode</t>
   </si>
@@ -426,7 +423,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,41 +440,30 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>